<commit_message>
Build before Create Author CSV video
This build of the project is one that has been created before the Create Author CSV video
</commit_message>
<xml_diff>
--- a/quotes.xlsx
+++ b/quotes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/grocottk70790_masseyhigh_school_nz/Documents/COM301/91902_Databases/01_Databases_Tutorial/91902_Support_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/grocottk70790_masseyhigh_school_nz/Documents/COM301/91902_Databases/01_Databases_Tutorial/L3_Practice_Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="469" documentId="13_ncr:40009_{9D8BBAB9-FE52-49AE-80E4-CBD616388BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{506CE86A-56A8-4732-8FBF-45C80DC26F8B}"/>
+  <xr:revisionPtr revIDLastSave="488" documentId="13_ncr:40009_{9D8BBAB9-FE52-49AE-80E4-CBD616388BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CF3620E-A841-4B6C-B618-BEB5519C0DC2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="334">
   <si>
     <t>misattributed-eleanor-roosevelt</t>
   </si>
@@ -5130,8 +5130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160C4483-0E1D-4CE7-ABDD-C5A3B5C40117}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7944,7 +7944,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8105,8 +8105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A597FD-ABA9-415B-B9D5-19AEDF24ABEE}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8345,15 +8345,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0F2601-016E-4EFA-8F38-3ABC1941B5D5}">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>321</v>
       </c>
@@ -8364,159 +8364,135 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>220</v>
+        <v>323</v>
       </c>
       <c r="E1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>223</v>
       </c>
-      <c r="D2" t="s">
-        <v>73</v>
+      <c r="D2">
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="F2">
-        <v>81</v>
-      </c>
-      <c r="G2">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>224</v>
       </c>
-      <c r="D3" t="s">
-        <v>75</v>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>225</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="D4">
+        <v>47</v>
       </c>
       <c r="E4">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F4">
-        <v>54</v>
-      </c>
-      <c r="G4">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>226</v>
       </c>
-      <c r="D5" t="s">
-        <v>78</v>
+      <c r="D5">
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F5">
-        <v>17</v>
-      </c>
-      <c r="G5">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>227</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
+      <c r="D6">
+        <v>47</v>
       </c>
       <c r="E6">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6">
-        <v>45</v>
-      </c>
-      <c r="G6">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>228</v>
       </c>
-      <c r="D7" t="s">
-        <v>221</v>
+      <c r="D7">
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="F7">
-        <v>79</v>
-      </c>
-      <c r="G7">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>229</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
+      <c r="D8">
+        <v>54</v>
       </c>
       <c r="E8">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F8">
-        <v>56</v>
-      </c>
-      <c r="G8">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>48</v>
       </c>
@@ -8526,17 +8502,14 @@
       <c r="C9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" t="s">
-        <v>82</v>
+      <c r="D9">
+        <v>27</v>
       </c>
       <c r="E9">
-        <v>27</v>
-      </c>
-      <c r="F9">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -8546,196 +8519,163 @@
       <c r="C10" t="s">
         <v>0</v>
       </c>
-      <c r="D10" t="s">
-        <v>139</v>
+      <c r="D10">
+        <v>90</v>
       </c>
       <c r="E10">
-        <v>90</v>
-      </c>
-      <c r="F10">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>232</v>
       </c>
-      <c r="D11" t="s">
-        <v>5</v>
+      <c r="D11">
+        <v>43</v>
       </c>
       <c r="E11">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F11">
-        <v>63</v>
-      </c>
-      <c r="G11">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>233</v>
       </c>
-      <c r="D12" t="s">
-        <v>18</v>
+      <c r="D12">
+        <v>54</v>
       </c>
       <c r="E12">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="F12">
-        <v>79</v>
-      </c>
-      <c r="G12">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>27</v>
       </c>
       <c r="B13" t="s">
         <v>234</v>
       </c>
-      <c r="D13" t="s">
-        <v>17</v>
+      <c r="D13">
+        <v>19</v>
       </c>
       <c r="E13">
+        <v>33</v>
+      </c>
+      <c r="F13">
         <v>19</v>
       </c>
-      <c r="F13">
-        <v>33</v>
-      </c>
-      <c r="G13">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>235</v>
       </c>
-      <c r="D14" t="s">
-        <v>87</v>
+      <c r="D14">
+        <v>77</v>
       </c>
       <c r="E14">
-        <v>77</v>
-      </c>
-      <c r="F14">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>236</v>
       </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15">
+      <c r="D15">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>237</v>
       </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16">
+      <c r="D16">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>238</v>
       </c>
-      <c r="D17" t="s">
-        <v>18</v>
+      <c r="D17">
+        <v>54</v>
       </c>
       <c r="E17">
-        <v>54</v>
-      </c>
-      <c r="F17">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>239</v>
       </c>
-      <c r="D18" t="s">
-        <v>90</v>
+      <c r="D18">
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="F18">
-        <v>46</v>
-      </c>
-      <c r="G18">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>240</v>
       </c>
-      <c r="D19" t="s">
-        <v>1</v>
+      <c r="D19">
+        <v>56</v>
       </c>
       <c r="E19">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="F19">
-        <v>33</v>
-      </c>
-      <c r="G19">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>241</v>
       </c>
-      <c r="D20" t="s">
-        <v>78</v>
+      <c r="D20">
+        <v>10</v>
       </c>
       <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -8745,51 +8685,42 @@
       <c r="C21" t="s">
         <v>96</v>
       </c>
-      <c r="D21" t="s">
-        <v>95</v>
+      <c r="D21">
+        <v>30</v>
       </c>
       <c r="E21">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="F21">
-        <v>54</v>
-      </c>
-      <c r="G21">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>243</v>
       </c>
-      <c r="D22" t="s">
-        <v>1</v>
+      <c r="D22">
+        <v>56</v>
       </c>
       <c r="E22">
-        <v>56</v>
-      </c>
-      <c r="F22">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>244</v>
       </c>
-      <c r="D23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23">
+      <c r="D23">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>41</v>
       </c>
@@ -8799,187 +8730,154 @@
       <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
-        <v>210</v>
+      <c r="D24">
+        <v>67</v>
       </c>
       <c r="E24">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="F24">
-        <v>49</v>
-      </c>
-      <c r="G24">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>246</v>
       </c>
-      <c r="D25" t="s">
-        <v>5</v>
+      <c r="D25">
+        <v>43</v>
       </c>
       <c r="E25">
-        <v>43</v>
-      </c>
-      <c r="F25">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>32</v>
       </c>
       <c r="B26" t="s">
         <v>247</v>
       </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26">
+      <c r="D26">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>248</v>
       </c>
-      <c r="D27" t="s">
-        <v>100</v>
+      <c r="D27">
+        <v>18</v>
       </c>
       <c r="E27">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="F27">
-        <v>54</v>
-      </c>
-      <c r="G27">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
         <v>249</v>
       </c>
-      <c r="D28" t="s">
-        <v>102</v>
+      <c r="D28">
+        <v>13</v>
       </c>
       <c r="E28">
-        <v>13</v>
-      </c>
-      <c r="F28">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>250</v>
       </c>
-      <c r="D29" t="s">
-        <v>18</v>
+      <c r="D29">
+        <v>54</v>
       </c>
       <c r="E29">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="F29">
-        <v>27</v>
-      </c>
-      <c r="G29">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>251</v>
       </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30">
+      <c r="D30">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
       <c r="B31" t="s">
         <v>252</v>
       </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31">
+      <c r="D31">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12</v>
       </c>
       <c r="B32" t="s">
         <v>253</v>
       </c>
-      <c r="D32" t="s">
-        <v>103</v>
+      <c r="D32">
+        <v>51</v>
       </c>
       <c r="E32">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="F32">
-        <v>71</v>
-      </c>
-      <c r="G32">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>68</v>
       </c>
-      <c r="D33" t="s">
-        <v>222</v>
+      <c r="D33">
+        <v>72</v>
       </c>
       <c r="E33">
-        <v>72</v>
-      </c>
-      <c r="F33">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
       <c r="B34" t="s">
         <v>254</v>
       </c>
-      <c r="D34" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34">
+      <c r="D34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>41</v>
       </c>
@@ -8989,54 +8887,45 @@
       <c r="C35" t="s">
         <v>106</v>
       </c>
-      <c r="D35" t="s">
-        <v>1</v>
+      <c r="D35">
+        <v>56</v>
       </c>
       <c r="E35">
-        <v>56</v>
-      </c>
-      <c r="F35">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>256</v>
       </c>
-      <c r="D36" t="s">
-        <v>107</v>
+      <c r="D36">
+        <v>20</v>
       </c>
       <c r="E36">
-        <v>20</v>
-      </c>
-      <c r="F36">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>257</v>
       </c>
-      <c r="D37" t="s">
-        <v>108</v>
+      <c r="D37">
+        <v>14</v>
       </c>
       <c r="E37">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F37">
-        <v>32</v>
-      </c>
-      <c r="G37">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>50</v>
       </c>
@@ -9046,170 +8935,140 @@
       <c r="C38" t="s">
         <v>110</v>
       </c>
-      <c r="D38" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38">
+      <c r="D38">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
         <v>259</v>
       </c>
-      <c r="D39" t="s">
-        <v>111</v>
+      <c r="D39">
+        <v>50</v>
       </c>
       <c r="E39">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F39">
-        <v>51</v>
-      </c>
-      <c r="G39">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>260</v>
       </c>
-      <c r="D40" t="s">
-        <v>78</v>
+      <c r="D40">
+        <v>10</v>
       </c>
       <c r="E40">
-        <v>10</v>
-      </c>
-      <c r="F40">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>261</v>
       </c>
-      <c r="D41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41">
+      <c r="D41">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>22</v>
       </c>
       <c r="B42" t="s">
         <v>262</v>
       </c>
-      <c r="D42" t="s">
-        <v>104</v>
+      <c r="D42">
+        <v>71</v>
       </c>
       <c r="E42">
+        <v>10</v>
+      </c>
+      <c r="F42">
         <v>71</v>
       </c>
-      <c r="F42">
-        <v>10</v>
-      </c>
-      <c r="G42">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>263</v>
       </c>
-      <c r="D43" t="s">
-        <v>78</v>
+      <c r="D43">
+        <v>10</v>
       </c>
       <c r="E43">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="F43">
-        <v>71</v>
-      </c>
-      <c r="G43">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>38</v>
       </c>
       <c r="B44" t="s">
         <v>264</v>
       </c>
-      <c r="D44" t="s">
-        <v>212</v>
+      <c r="D44">
+        <v>84</v>
       </c>
       <c r="E44">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="F44">
-        <v>8</v>
-      </c>
-      <c r="G44">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>38</v>
       </c>
       <c r="B45" t="s">
         <v>265</v>
       </c>
-      <c r="D45" t="s">
-        <v>114</v>
+      <c r="D45">
+        <v>35</v>
       </c>
       <c r="E45">
-        <v>35</v>
-      </c>
-      <c r="F45">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
         <v>266</v>
       </c>
-      <c r="D46" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46">
+      <c r="D46">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>38</v>
       </c>
       <c r="B47" t="s">
         <v>267</v>
       </c>
-      <c r="D47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47">
+      <c r="D47">
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>38</v>
       </c>
@@ -9219,82 +9078,67 @@
       <c r="C48" t="s">
         <v>4</v>
       </c>
-      <c r="D48" t="s">
-        <v>1</v>
+      <c r="D48">
+        <v>56</v>
       </c>
       <c r="E48">
-        <v>56</v>
-      </c>
-      <c r="F48">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>40</v>
       </c>
       <c r="B49" t="s">
         <v>269</v>
       </c>
-      <c r="D49" t="s">
-        <v>115</v>
+      <c r="D49">
+        <v>42</v>
       </c>
       <c r="E49">
-        <v>42</v>
-      </c>
-      <c r="F49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>27</v>
       </c>
       <c r="B50" t="s">
         <v>270</v>
       </c>
-      <c r="D50" t="s">
-        <v>319</v>
+      <c r="D50">
+        <v>9</v>
       </c>
       <c r="E50">
-        <v>9</v>
-      </c>
-      <c r="F50">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>30</v>
       </c>
       <c r="B51" t="s">
         <v>271</v>
       </c>
-      <c r="D51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51">
+      <c r="D51">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>31</v>
       </c>
       <c r="B52" t="s">
         <v>272</v>
       </c>
-      <c r="D52" t="s">
-        <v>86</v>
+      <c r="D52">
+        <v>33</v>
       </c>
       <c r="E52">
-        <v>33</v>
-      </c>
-      <c r="F52">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>14</v>
       </c>
@@ -9304,17 +9148,14 @@
       <c r="C53" t="s">
         <v>116</v>
       </c>
-      <c r="D53" t="s">
-        <v>117</v>
+      <c r="D53">
+        <v>31</v>
       </c>
       <c r="E53">
-        <v>31</v>
-      </c>
-      <c r="F53">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>38</v>
       </c>
@@ -9324,51 +9165,42 @@
       <c r="C54" t="s">
         <v>4</v>
       </c>
-      <c r="D54" t="s">
-        <v>1</v>
+      <c r="D54">
+        <v>56</v>
       </c>
       <c r="E54">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F54">
-        <v>37</v>
-      </c>
-      <c r="G54">
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
       <c r="B55" t="s">
         <v>275</v>
       </c>
-      <c r="D55" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55">
+      <c r="D55">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>24</v>
       </c>
       <c r="B56" t="s">
         <v>276</v>
       </c>
-      <c r="D56" t="s">
-        <v>78</v>
+      <c r="D56">
+        <v>10</v>
       </c>
       <c r="E56">
-        <v>10</v>
-      </c>
-      <c r="F56">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -9378,555 +9210,456 @@
       <c r="C57" t="s">
         <v>9</v>
       </c>
-      <c r="D57" t="s">
-        <v>138</v>
+      <c r="D57">
+        <v>34</v>
       </c>
       <c r="E57">
-        <v>34</v>
-      </c>
-      <c r="F57">
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>44</v>
       </c>
       <c r="B58" t="s">
         <v>278</v>
       </c>
-      <c r="D58" t="s">
-        <v>119</v>
+      <c r="D58">
+        <v>23</v>
       </c>
       <c r="E58">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F58">
-        <v>56</v>
-      </c>
-      <c r="G58">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>16</v>
       </c>
       <c r="B59" t="s">
         <v>279</v>
       </c>
-      <c r="D59" t="s">
-        <v>78</v>
+      <c r="D59">
+        <v>10</v>
       </c>
       <c r="E59">
-        <v>10</v>
-      </c>
-      <c r="F59">
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>25</v>
       </c>
       <c r="B60" t="s">
         <v>280</v>
       </c>
-      <c r="D60" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60">
+      <c r="D60">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>19</v>
       </c>
       <c r="B61" t="s">
         <v>281</v>
       </c>
-      <c r="D61" t="s">
-        <v>8</v>
+      <c r="D61">
+        <v>47</v>
       </c>
       <c r="E61">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F61">
-        <v>54</v>
-      </c>
-      <c r="G61">
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
       <c r="B62" t="s">
         <v>282</v>
       </c>
-      <c r="D62" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62">
+      <c r="D62">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>46</v>
       </c>
       <c r="B63" t="s">
         <v>283</v>
       </c>
-      <c r="D63" t="s">
-        <v>210</v>
+      <c r="D63">
+        <v>67</v>
       </c>
       <c r="E63">
-        <v>67</v>
-      </c>
-      <c r="F63">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>46</v>
       </c>
       <c r="B64" t="s">
         <v>284</v>
       </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64">
+      <c r="D64">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>8</v>
       </c>
       <c r="B65" t="s">
         <v>285</v>
       </c>
-      <c r="D65" t="s">
-        <v>1</v>
-      </c>
-      <c r="E65">
+      <c r="D65">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>29</v>
       </c>
       <c r="B66" t="s">
         <v>286</v>
       </c>
-      <c r="D66" t="s">
-        <v>121</v>
+      <c r="D66">
+        <v>82</v>
       </c>
       <c r="E66">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="F66">
-        <v>55</v>
-      </c>
-      <c r="G66">
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>27</v>
       </c>
       <c r="B67" t="s">
         <v>287</v>
       </c>
-      <c r="D67" t="s">
-        <v>18</v>
+      <c r="D67">
+        <v>54</v>
       </c>
       <c r="E67">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="F67">
-        <v>20</v>
-      </c>
-      <c r="G67">
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>16</v>
       </c>
       <c r="B68" t="s">
         <v>288</v>
       </c>
-      <c r="D68" t="s">
-        <v>123</v>
+      <c r="D68">
+        <v>37</v>
       </c>
       <c r="E68">
-        <v>37</v>
-      </c>
-      <c r="F68">
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>43</v>
       </c>
       <c r="B69" t="s">
         <v>289</v>
       </c>
-      <c r="D69" t="s">
-        <v>18</v>
+      <c r="D69">
+        <v>54</v>
       </c>
       <c r="E69">
-        <v>54</v>
-      </c>
-      <c r="F69">
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>39</v>
       </c>
       <c r="B70" t="s">
         <v>290</v>
       </c>
-      <c r="D70" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70">
+      <c r="D70">
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>12</v>
       </c>
       <c r="B71" t="s">
         <v>71</v>
       </c>
-      <c r="D71" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71">
+      <c r="D71">
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3</v>
       </c>
       <c r="B72" t="s">
         <v>291</v>
       </c>
-      <c r="D72" t="s">
-        <v>86</v>
+      <c r="D72">
+        <v>33</v>
       </c>
       <c r="E72">
-        <v>33</v>
-      </c>
-      <c r="F72">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9</v>
       </c>
       <c r="B73" t="s">
         <v>292</v>
       </c>
-      <c r="D73" t="s">
-        <v>5</v>
-      </c>
-      <c r="E73">
+      <c r="D73">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>47</v>
       </c>
       <c r="B74" t="s">
         <v>293</v>
       </c>
-      <c r="D74" t="s">
-        <v>5</v>
+      <c r="D74">
+        <v>43</v>
       </c>
       <c r="E74">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="F74">
-        <v>64</v>
-      </c>
-      <c r="G74">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>69</v>
       </c>
-      <c r="D75" t="s">
-        <v>5</v>
+      <c r="D75">
+        <v>43</v>
       </c>
       <c r="E75">
-        <v>43</v>
-      </c>
-      <c r="F75">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>26</v>
       </c>
       <c r="B76" t="s">
         <v>294</v>
       </c>
-      <c r="D76" t="s">
-        <v>78</v>
+      <c r="D76">
+        <v>10</v>
       </c>
       <c r="E76">
-        <v>10</v>
-      </c>
-      <c r="F76">
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>20</v>
       </c>
       <c r="B77" t="s">
         <v>295</v>
       </c>
-      <c r="D77" t="s">
-        <v>5</v>
-      </c>
-      <c r="E77">
+      <c r="D77">
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>34</v>
       </c>
       <c r="B78" t="s">
         <v>296</v>
       </c>
-      <c r="D78" t="s">
-        <v>127</v>
+      <c r="D78">
+        <v>7</v>
       </c>
       <c r="E78">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F78">
-        <v>22</v>
-      </c>
-      <c r="G78">
         <v>66</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>49</v>
       </c>
       <c r="B79" t="s">
         <v>70</v>
       </c>
-      <c r="D79" t="s">
-        <v>5</v>
+      <c r="D79">
+        <v>43</v>
       </c>
       <c r="E79">
-        <v>43</v>
-      </c>
-      <c r="F79">
         <v>41</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>6</v>
       </c>
       <c r="B80" t="s">
         <v>297</v>
       </c>
-      <c r="D80" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80">
+      <c r="D80">
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>39</v>
       </c>
       <c r="B81" t="s">
         <v>298</v>
       </c>
-      <c r="D81" t="s">
-        <v>78</v>
+      <c r="D81">
+        <v>10</v>
       </c>
       <c r="E81">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F81">
-        <v>17</v>
-      </c>
-      <c r="G81">
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1</v>
       </c>
       <c r="B82" t="s">
         <v>299</v>
       </c>
-      <c r="D82" t="s">
-        <v>13</v>
-      </c>
-      <c r="E82">
+      <c r="D82">
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>31</v>
       </c>
       <c r="B83" t="s">
         <v>300</v>
       </c>
-      <c r="D83" t="s">
-        <v>5</v>
+      <c r="D83">
+        <v>43</v>
       </c>
       <c r="E83">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F83">
-        <v>56</v>
-      </c>
-      <c r="G83">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>27</v>
       </c>
       <c r="B84" t="s">
         <v>301</v>
       </c>
-      <c r="D84" t="s">
-        <v>14</v>
-      </c>
-      <c r="E84">
+      <c r="D84">
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>31</v>
       </c>
       <c r="B85" t="s">
         <v>302</v>
       </c>
-      <c r="D85" t="s">
-        <v>78</v>
+      <c r="D85">
+        <v>10</v>
       </c>
       <c r="E85">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F85">
-        <v>52</v>
-      </c>
-      <c r="G85">
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>31</v>
       </c>
       <c r="B86" t="s">
         <v>303</v>
       </c>
-      <c r="D86" t="s">
-        <v>79</v>
+      <c r="D86">
+        <v>17</v>
       </c>
       <c r="E86">
-        <v>17</v>
-      </c>
-      <c r="F86">
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>8</v>
       </c>
       <c r="B87" t="s">
         <v>304</v>
       </c>
-      <c r="D87" t="s">
-        <v>129</v>
+      <c r="D87">
+        <v>5</v>
       </c>
       <c r="E87">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="F87">
-        <v>71</v>
-      </c>
-      <c r="G87">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>8</v>
       </c>
       <c r="B88" t="s">
         <v>305</v>
       </c>
-      <c r="D88" t="s">
-        <v>15</v>
-      </c>
-      <c r="E88">
+      <c r="D88">
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>39</v>
       </c>
       <c r="B89" t="s">
         <v>306</v>
       </c>
-      <c r="D89" t="s">
-        <v>107</v>
+      <c r="D89">
+        <v>20</v>
       </c>
       <c r="E89">
-        <v>20</v>
-      </c>
-      <c r="F89">
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>39</v>
       </c>
@@ -9936,228 +9669,186 @@
       <c r="C90" t="s">
         <v>130</v>
       </c>
-      <c r="D90" t="s">
-        <v>16</v>
-      </c>
-      <c r="E90">
+      <c r="D90">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>8</v>
       </c>
       <c r="B91" t="s">
         <v>308</v>
       </c>
-      <c r="D91" t="s">
-        <v>131</v>
+      <c r="D91">
+        <v>16</v>
       </c>
       <c r="E91">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F91">
-        <v>28</v>
-      </c>
-      <c r="G91">
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>27</v>
       </c>
       <c r="B92" t="s">
         <v>309</v>
       </c>
-      <c r="D92" t="s">
-        <v>16</v>
-      </c>
-      <c r="E92">
+      <c r="D92">
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>33</v>
       </c>
       <c r="B93" t="s">
         <v>310</v>
       </c>
-      <c r="D93" t="s">
-        <v>107</v>
+      <c r="D93">
+        <v>20</v>
       </c>
       <c r="E93">
-        <v>20</v>
-      </c>
-      <c r="F93">
         <v>54</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>28</v>
       </c>
       <c r="B94" t="s">
         <v>311</v>
       </c>
-      <c r="D94" t="s">
-        <v>133</v>
+      <c r="D94">
+        <v>4</v>
       </c>
       <c r="E94">
-        <v>4</v>
-      </c>
-      <c r="F94">
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>13</v>
       </c>
       <c r="B95" t="s">
         <v>312</v>
       </c>
-      <c r="D95" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95">
+      <c r="D95">
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>36</v>
       </c>
       <c r="B96" t="s">
         <v>313</v>
       </c>
-      <c r="D96" t="s">
-        <v>18</v>
-      </c>
-      <c r="E96">
+      <c r="D96">
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>23</v>
       </c>
       <c r="B97" t="s">
         <v>314</v>
       </c>
-      <c r="D97" t="s">
-        <v>18</v>
+      <c r="D97">
+        <v>54</v>
       </c>
       <c r="E97">
-        <v>54</v>
-      </c>
-      <c r="F97">
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>37</v>
       </c>
       <c r="B98" t="s">
         <v>315</v>
       </c>
-      <c r="D98" t="s">
-        <v>78</v>
+      <c r="D98">
+        <v>10</v>
       </c>
       <c r="E98">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F98">
-        <v>13</v>
-      </c>
-      <c r="G98">
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>39</v>
       </c>
       <c r="B99" t="s">
         <v>316</v>
       </c>
-      <c r="D99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E99">
+      <c r="D99">
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>12</v>
       </c>
       <c r="B100" t="s">
         <v>317</v>
       </c>
-      <c r="D100" t="s">
-        <v>8</v>
-      </c>
-      <c r="E100">
+      <c r="D100">
         <v>47</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>22</v>
       </c>
       <c r="B101" t="s">
         <v>318</v>
       </c>
-      <c r="D101" t="s">
-        <v>78</v>
+      <c r="D101">
+        <v>10</v>
       </c>
       <c r="E101">
-        <v>10</v>
-      </c>
-      <c r="F101">
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>47</v>
       </c>
       <c r="B102" t="s">
         <v>205</v>
       </c>
-      <c r="D102" t="s">
-        <v>8</v>
+      <c r="D102">
+        <v>47</v>
       </c>
       <c r="E102">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F102">
-        <v>21</v>
-      </c>
-      <c r="G102">
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>47</v>
       </c>
       <c r="B103" t="s">
         <v>209</v>
       </c>
-      <c r="D103" t="s">
-        <v>18</v>
+      <c r="D103">
+        <v>54</v>
       </c>
       <c r="E103">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F103">
-        <v>67</v>
-      </c>
-      <c r="G103">
         <v>11</v>
       </c>
     </row>
@@ -10170,8 +9861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA2C2B3-88B9-4171-89A6-7E946B9FCA98}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Build at Checkpoint 1
This is a build of the database that has been created around the time of the first checkpoint (Checkpoint 1).
</commit_message>
<xml_diff>
--- a/quotes.xlsx
+++ b/quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/grocottk70790_masseyhigh_school_nz/Documents/COM301/91902_Databases/01_Databases_Tutorial/L3_Practice_Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="13_ncr:40009_{9D8BBAB9-FE52-49AE-80E4-CBD616388BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CF3620E-A841-4B6C-B618-BEB5519C0DC2}"/>
+  <xr:revisionPtr revIDLastSave="496" documentId="13_ncr:40009_{9D8BBAB9-FE52-49AE-80E4-CBD616388BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73438EE2-4EFC-4FC1-A2A8-7B44B5265808}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="334">
   <si>
     <t>misattributed-eleanor-roosevelt</t>
   </si>
@@ -5904,7 +5904,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8105,7 +8105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A597FD-ABA9-415B-B9D5-19AEDF24ABEE}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -9859,1195 +9859,1207 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA2C2B3-88B9-4171-89A6-7E946B9FCA98}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s">
-        <v>321</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>330</v>
       </c>
       <c r="E1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>164</v>
       </c>
+      <c r="C2">
+        <v>1879</v>
+      </c>
       <c r="D2">
-        <v>1879</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>17</v>
       </c>
       <c r="G2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3">
+        <v>1824</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4">
+        <v>1809</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5">
+        <v>1899</v>
+      </c>
+      <c r="D5">
         <v>17</v>
       </c>
-      <c r="H2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>164</v>
       </c>
-      <c r="D3">
-        <v>1824</v>
-      </c>
-      <c r="E3">
+      <c r="C6">
+        <v>1869</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="H3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7">
+        <v>1905</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>164</v>
       </c>
-      <c r="D4">
-        <v>1809</v>
-      </c>
-      <c r="E4">
+      <c r="C8">
+        <v>1945</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9">
+        <v>1898</v>
+      </c>
+      <c r="D9">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10">
+        <v>1920</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5">
+      <c r="G10">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>164</v>
       </c>
-      <c r="D5">
+      <c r="C11">
+        <v>1922</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12">
+        <v>1952</v>
+      </c>
+      <c r="D12">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13">
+        <v>1904</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14">
+        <v>1894</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>19</v>
+      </c>
+      <c r="G14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15">
+        <v>1884</v>
+      </c>
+      <c r="D15">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16">
+        <v>1928</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>17</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17">
         <v>1899</v>
       </c>
-      <c r="E5">
+      <c r="D17">
         <v>17</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6">
-        <v>1869</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7">
-        <v>1905</v>
-      </c>
-      <c r="E7">
-        <v>13</v>
-      </c>
-      <c r="F7">
-        <v>17</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8">
-        <v>1945</v>
-      </c>
-      <c r="E8">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>17</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9">
-        <v>1898</v>
-      </c>
-      <c r="E9">
-        <v>16</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10">
-        <v>1920</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>17</v>
-      </c>
-      <c r="G10">
-        <v>19</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11">
-        <v>1922</v>
-      </c>
-      <c r="E11">
-        <v>17</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12">
-        <v>1952</v>
-      </c>
-      <c r="E12">
-        <v>17</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>164</v>
-      </c>
-      <c r="D13">
-        <v>1904</v>
-      </c>
-      <c r="E13">
-        <v>17</v>
-      </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="H13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>164</v>
-      </c>
-      <c r="D14">
-        <v>1894</v>
-      </c>
-      <c r="E14">
-        <v>17</v>
-      </c>
-      <c r="G14">
-        <v>19</v>
-      </c>
-      <c r="H14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>165</v>
-      </c>
-      <c r="D15">
-        <v>1884</v>
-      </c>
-      <c r="E15">
-        <v>17</v>
-      </c>
-      <c r="G15">
-        <v>7</v>
-      </c>
-      <c r="H15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16">
-        <v>1928</v>
-      </c>
-      <c r="E16">
-        <v>12</v>
-      </c>
-      <c r="F16">
-        <v>17</v>
-      </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D17">
-        <v>1899</v>
       </c>
       <c r="E17">
         <v>17</v>
       </c>
       <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" t="s">
         <v>164</v>
       </c>
+      <c r="C18">
+        <v>1884</v>
+      </c>
       <c r="D18">
-        <v>1884</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>6</v>
       </c>
       <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19">
+        <v>1942</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20">
+        <v>1856</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>17</v>
+      </c>
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21">
+        <v>1937</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>6</v>
       </c>
-      <c r="G18">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22">
+        <v>1819</v>
+      </c>
+      <c r="D22">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23">
+        <v>1948</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24">
+        <v>1926</v>
+      </c>
+      <c r="D24">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25">
+        <v>1949</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26">
+        <v>1880</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27">
+        <v>1919</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28">
+        <v>1965</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29">
+        <v>1860</v>
+      </c>
+      <c r="D29">
+        <v>16</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30">
+        <v>1892</v>
+      </c>
+      <c r="D30">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31">
+        <v>1924</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32">
+        <v>1775</v>
+      </c>
+      <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33">
+        <v>1936</v>
+      </c>
+      <c r="D33">
+        <v>17</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>22</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34">
+        <v>1942</v>
+      </c>
+      <c r="D34">
+        <v>17</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>12</v>
+      </c>
+      <c r="G34">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35">
+        <v>1940</v>
+      </c>
+      <c r="D35">
+        <v>16</v>
+      </c>
+      <c r="E35">
+        <v>17</v>
+      </c>
+      <c r="F35">
+        <v>25</v>
+      </c>
+      <c r="G35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36">
+        <v>1899</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37">
+        <v>1965</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>17</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B38" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38">
+        <v>1918</v>
+      </c>
+      <c r="D38">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39">
+        <v>1926</v>
+      </c>
+      <c r="D39">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>164</v>
       </c>
-      <c r="D19">
-        <v>1942</v>
-      </c>
-      <c r="E19">
+      <c r="C40">
+        <v>1835</v>
+      </c>
+      <c r="D40">
         <v>17</v>
       </c>
-      <c r="G19">
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
         <v>4</v>
       </c>
-      <c r="H19">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41">
+        <v>1929</v>
+      </c>
+      <c r="D41">
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>21</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42">
+        <v>1910</v>
+      </c>
+      <c r="D42">
+        <v>11</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
+        <v>13</v>
+      </c>
+      <c r="G42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43">
+        <v>1904</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>164</v>
       </c>
-      <c r="D20">
-        <v>1856</v>
-      </c>
-      <c r="E20">
-        <v>8</v>
-      </c>
-      <c r="F20">
+      <c r="C44">
+        <v>1803</v>
+      </c>
+      <c r="D44">
         <v>17</v>
       </c>
-      <c r="G20">
-        <v>18</v>
-      </c>
-      <c r="H20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>19</v>
+      </c>
+      <c r="G44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45">
+        <v>1973</v>
+      </c>
+      <c r="D45">
+        <v>17</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>164</v>
       </c>
-      <c r="D21">
-        <v>1937</v>
-      </c>
-      <c r="E21">
+      <c r="C46">
+        <v>1945</v>
+      </c>
+      <c r="D46">
         <v>17</v>
       </c>
-      <c r="G21">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
         <v>6</v>
       </c>
-      <c r="H21">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47">
+        <v>1962</v>
+      </c>
+      <c r="D47">
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>165</v>
-      </c>
-      <c r="D22">
-        <v>1819</v>
-      </c>
-      <c r="E22">
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48">
+        <v>1948</v>
+      </c>
+      <c r="D48">
         <v>16</v>
       </c>
-      <c r="G22">
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
         <v>4</v>
       </c>
-      <c r="H22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>164</v>
       </c>
-      <c r="D23">
-        <v>1948</v>
-      </c>
-      <c r="E23">
+      <c r="C49">
+        <v>1847</v>
+      </c>
+      <c r="D49">
         <v>17</v>
       </c>
-      <c r="G23">
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>9</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50">
+        <v>1880</v>
+      </c>
+      <c r="D50">
+        <v>17</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51">
+        <v>1872</v>
+      </c>
+      <c r="D51">
+        <v>16</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52">
+        <v>1869</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>165</v>
-      </c>
-      <c r="D24">
-        <v>1926</v>
-      </c>
-      <c r="E24">
-        <v>17</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>164</v>
-      </c>
-      <c r="D25">
-        <v>1949</v>
-      </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
-      <c r="G25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>165</v>
-      </c>
-      <c r="D26">
-        <v>1880</v>
-      </c>
-      <c r="E26">
-        <v>17</v>
-      </c>
-      <c r="G26">
-        <v>4</v>
-      </c>
-      <c r="H26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27">
-        <v>1919</v>
-      </c>
-      <c r="E27">
-        <v>17</v>
-      </c>
-      <c r="G27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>165</v>
-      </c>
-      <c r="D28">
-        <v>1965</v>
-      </c>
-      <c r="E28">
-        <v>16</v>
-      </c>
-      <c r="G28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>164</v>
-      </c>
-      <c r="D29">
-        <v>1860</v>
-      </c>
-      <c r="E29">
-        <v>16</v>
-      </c>
-      <c r="G29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30">
-        <v>1892</v>
-      </c>
-      <c r="E30">
-        <v>14</v>
-      </c>
-      <c r="F30">
-        <v>16</v>
-      </c>
-      <c r="G30">
-        <v>4</v>
-      </c>
-      <c r="H30">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>164</v>
-      </c>
-      <c r="D31">
-        <v>1924</v>
-      </c>
-      <c r="E31">
-        <v>17</v>
-      </c>
-      <c r="F31">
-        <v>5</v>
-      </c>
-      <c r="G31">
-        <v>4</v>
-      </c>
-      <c r="H31">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s">
-        <v>165</v>
-      </c>
-      <c r="D32">
-        <v>1775</v>
-      </c>
-      <c r="E32">
-        <v>16</v>
-      </c>
-      <c r="G32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>164</v>
-      </c>
-      <c r="D33">
-        <v>1936</v>
-      </c>
-      <c r="E33">
-        <v>17</v>
-      </c>
-      <c r="G33">
-        <v>22</v>
-      </c>
-      <c r="H33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s">
-        <v>164</v>
-      </c>
-      <c r="D34">
-        <v>1942</v>
-      </c>
-      <c r="E34">
-        <v>17</v>
-      </c>
-      <c r="G34">
-        <v>12</v>
-      </c>
-      <c r="H34">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>164</v>
-      </c>
-      <c r="D35">
-        <v>1940</v>
-      </c>
-      <c r="E35">
-        <v>16</v>
-      </c>
-      <c r="F35">
-        <v>17</v>
-      </c>
-      <c r="G35">
-        <v>25</v>
-      </c>
-      <c r="H35">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36">
-        <v>35</v>
-      </c>
-      <c r="C36" t="s">
-        <v>164</v>
-      </c>
-      <c r="D36">
-        <v>1899</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36">
-        <v>15</v>
-      </c>
-      <c r="G36">
-        <v>4</v>
-      </c>
-      <c r="H36">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37">
-        <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>164</v>
-      </c>
-      <c r="D37">
-        <v>1965</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>17</v>
-      </c>
-      <c r="G37">
-        <v>4</v>
-      </c>
-      <c r="H37">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38">
-        <v>37</v>
-      </c>
-      <c r="C38" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38">
-        <v>1918</v>
-      </c>
-      <c r="E38">
-        <v>17</v>
-      </c>
-      <c r="G38">
-        <v>4</v>
-      </c>
-      <c r="H38">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39">
-        <v>38</v>
-      </c>
-      <c r="C39" t="s">
-        <v>165</v>
-      </c>
-      <c r="D39">
-        <v>1926</v>
-      </c>
-      <c r="E39">
-        <v>17</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40">
-        <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D40">
-        <v>1835</v>
-      </c>
-      <c r="E40">
-        <v>17</v>
-      </c>
-      <c r="G40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <v>40</v>
-      </c>
-      <c r="C41" t="s">
-        <v>164</v>
-      </c>
-      <c r="D41">
-        <v>1929</v>
-      </c>
-      <c r="E41">
-        <v>17</v>
-      </c>
-      <c r="G41">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42">
-        <v>1910</v>
-      </c>
-      <c r="E42">
-        <v>11</v>
-      </c>
-      <c r="F42">
-        <v>7</v>
-      </c>
-      <c r="G42">
-        <v>13</v>
-      </c>
-      <c r="H42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>164</v>
-      </c>
-      <c r="D43">
-        <v>1904</v>
-      </c>
-      <c r="E43">
-        <v>4</v>
-      </c>
-      <c r="G43">
-        <v>19</v>
-      </c>
-      <c r="H43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44">
-        <v>43</v>
-      </c>
-      <c r="C44" t="s">
-        <v>164</v>
-      </c>
-      <c r="D44">
-        <v>1803</v>
-      </c>
-      <c r="E44">
-        <v>17</v>
-      </c>
-      <c r="G44">
-        <v>19</v>
-      </c>
-      <c r="H44">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45">
-        <v>44</v>
-      </c>
-      <c r="C45" t="s">
-        <v>165</v>
-      </c>
-      <c r="D45">
-        <v>1973</v>
-      </c>
-      <c r="E45">
-        <v>17</v>
-      </c>
-      <c r="G45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46">
-        <v>45</v>
-      </c>
-      <c r="C46" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46">
-        <v>1945</v>
-      </c>
-      <c r="E46">
-        <v>17</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47">
-        <v>46</v>
-      </c>
-      <c r="C47" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47">
-        <v>1962</v>
-      </c>
-      <c r="E47">
-        <v>17</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>164</v>
-      </c>
-      <c r="D48">
-        <v>1948</v>
-      </c>
-      <c r="E48">
-        <v>16</v>
-      </c>
-      <c r="G48">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>164</v>
-      </c>
-      <c r="D49">
-        <v>1847</v>
-      </c>
-      <c r="E49">
-        <v>17</v>
-      </c>
-      <c r="G49">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50">
-        <v>49</v>
-      </c>
-      <c r="C50" t="s">
-        <v>164</v>
-      </c>
-      <c r="D50">
-        <v>1880</v>
-      </c>
-      <c r="E50">
-        <v>17</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>40</v>
-      </c>
-      <c r="B51">
-        <v>50</v>
-      </c>
-      <c r="C51" t="s">
-        <v>164</v>
-      </c>
-      <c r="D51">
-        <v>1872</v>
-      </c>
-      <c r="E51">
-        <v>16</v>
-      </c>
-      <c r="G51">
-        <v>3</v>
-      </c>
-      <c r="H51">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>206</v>
-      </c>
-      <c r="B52">
-        <v>51</v>
-      </c>
-      <c r="C52" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52">
-        <v>1869</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
-      </c>
       <c r="G52">
-        <v>4</v>
-      </c>
-      <c r="H52">
         <v>20</v>
       </c>
     </row>

</xml_diff>